<commit_message>
Se configura envio de correo y queda funcional, pendiente informacion adicional al momento de atender el turno
</commit_message>
<xml_diff>
--- a/DB/reporte_turnos_diario.xlsx
+++ b/DB/reporte_turnos_diario.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\turnero\DB\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CD15A5-708A-44D6-B61F-E622FB3FF3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,7 +40,7 @@
     <t>laura</t>
   </si>
   <si>
-    <t>2024-09-09</t>
+    <t>2024-09-12</t>
   </si>
   <si>
     <t>rocio</t>
@@ -67,8 +61,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,21 +99,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +143,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -191,7 +177,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -226,10 +211,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -402,16 +386,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +416,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>2</v>
       </c>
@@ -445,19 +427,19 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E2">
-        <v>1182.6429000000001</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <v>14</v>
       </c>
       <c r="G2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>3</v>
       </c>
@@ -468,24 +450,24 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>1443.6667</v>
+        <v>5.3333</v>
       </c>
       <c r="F3">
         <v>14</v>
       </c>
       <c r="G3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="E4">
-        <v>1303.1153999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.7778</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -493,28 +475,28 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10">
-        <v>1303.1153999999999</v>
+        <v>5.7778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se mejora apariencia del informe excel de reporte
</commit_message>
<xml_diff>
--- a/DB/reporte_turnos_diario.xlsx
+++ b/DB/reporte_turnos_diario.xlsx
@@ -1,25 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\turnero\DB\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132A0710-2A33-4B6F-BF70-751BE884AD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-28920" yWindow="-1095" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+  <si>
+    <t>AGENCIA CATASTRAL DE CUNDINAMARCA</t>
+  </si>
+  <si>
+    <t>INFORME DE RENDIMIENTOS ATENCIÓN DE USUARIOS</t>
+  </si>
   <si>
     <t>Usuario ID</t>
   </si>
   <si>
-    <t>Ventanilla</t>
+    <t>Funcionario</t>
   </si>
   <si>
     <t>Fecha</t>
@@ -28,7 +40,7 @@
     <t>Turnos Atendidos</t>
   </si>
   <si>
-    <t>Tiempo Promedio (minutos)</t>
+    <t>Tiempo Promedio (espera mn)</t>
   </si>
   <si>
     <t>Hora Pico</t>
@@ -61,9 +73,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,21 +119,85 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>898519</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>125940</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="49550310_598832710562102_5995102219237874750_n.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="47625"/>
+          <a:ext cx="850894" cy="268815"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -143,7 +235,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -177,6 +269,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -211,9 +304,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,120 +480,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="7" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
         <v>6</v>
       </c>
-      <c r="E2">
+      <c r="E4">
         <v>6</v>
       </c>
-      <c r="F2">
+      <c r="F4">
         <v>14</v>
       </c>
-      <c r="G2">
+      <c r="G4">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="E3">
-        <v>5.3333</v>
-      </c>
-      <c r="F3">
+      <c r="E5">
+        <v>5.3333000000000004</v>
+      </c>
+      <c r="F5">
         <v>14</v>
       </c>
-      <c r="G3">
+      <c r="G5">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="E4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6">
         <v>5.7778</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
         <v>5.7778</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>